<commit_message>
## 4 Initiative 3: User Experience and Secondary Features
</commit_message>
<xml_diff>
--- a/Documents/Product Backlog.xlsx
+++ b/Documents/Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\DeathFeePlanner\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC011AD0-4528-4393-AD16-CC7ACBB3D6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB3908A-E0F8-45B6-B9B5-8C587016C327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,9 +195,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -500,143 +507,146 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1128,10 +1138,10 @@
       <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="42"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
@@ -1150,27 +1160,27 @@
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
@@ -1182,10 +1192,10 @@
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="27" t="s">
         <v>51</v>
       </c>
       <c r="D6" s="16">
@@ -1194,10 +1204,10 @@
       <c r="E6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="28" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="1"/>
@@ -1208,16 +1218,16 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="16">
         <v>2</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="37"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1226,14 +1236,14 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="16">
         <v>3</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1242,14 +1252,14 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="16">
         <v>4</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="37"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1258,14 +1268,14 @@
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="16">
         <v>5</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1288,14 +1298,14 @@
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="17"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="40"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1304,12 +1314,12 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="17"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="40"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1318,12 +1328,12 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="17"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="40"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="31"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1332,12 +1342,12 @@
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="17"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="40"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1346,12 +1356,12 @@
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="17"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="31"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1374,14 +1384,14 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="16"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="37"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1390,12 +1400,12 @@
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="16"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="37"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1404,12 +1414,12 @@
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="16"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="37"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1418,12 +1428,12 @@
       <c r="M20" s="1"/>
     </row>
     <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="16"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="37"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1432,12 +1442,12 @@
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="16"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="37"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1460,14 +1470,14 @@
       <c r="M23" s="1"/>
     </row>
     <row r="24" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="39"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="17"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="31"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1476,12 +1486,12 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="38"/>
-      <c r="C25" s="39"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="17"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="40"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="31"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1490,12 +1500,12 @@
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="17"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="40"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="31"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1504,12 +1514,12 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="17"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="40"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1518,12 +1528,12 @@
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="17"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="40"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2019,12 +2029,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="G18:G22"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="C24:C28"/>
     <mergeCell ref="G24:G28"/>
@@ -2038,6 +2042,12 @@
     <mergeCell ref="F6:F10"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="F18:F22"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="G18:G22"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2057,8 +2067,8 @@
   </sheetPr>
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2084,51 +2094,51 @@
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:14" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -2147,10 +2157,10 @@
       <c r="C7" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
@@ -2168,10 +2178,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="27" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="16">
@@ -2180,13 +2190,13 @@
       <c r="E8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="28" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="1"/>
@@ -2197,17 +2207,17 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="16">
         <v>2</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="37"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="28"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -2216,17 +2226,17 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="16">
         <v>3</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="37"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="28"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2235,17 +2245,17 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="16">
         <v>4</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="37"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -2254,15 +2264,15 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="36"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="16">
         <v>5</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="37"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -2286,10 +2296,10 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="17">
@@ -2298,13 +2308,13 @@
       <c r="E14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="31" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="1"/>
@@ -2315,17 +2325,17 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="39"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
       <c r="D15" s="17">
         <v>2</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="40"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -2334,17 +2344,17 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="17">
         <v>3</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="40"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2353,17 +2363,17 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="17">
         <v>4</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="31"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2372,15 +2382,15 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="17">
         <v>5</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="40"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="31"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2404,10 +2414,10 @@
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="27" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="16">
@@ -2416,13 +2426,13 @@
       <c r="E20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="28" t="s">
         <v>34</v>
       </c>
       <c r="I20" s="1"/>
@@ -2433,17 +2443,17 @@
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="16">
         <v>2</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="37"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2452,17 +2462,17 @@
       <c r="N21" s="1"/>
     </row>
     <row r="22" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="36"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="16">
         <v>3</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="37"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2471,17 +2481,17 @@
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="16">
         <v>4</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="22"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="37"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2490,15 +2500,15 @@
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="16">
         <v>5</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="37"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2522,10 +2532,10 @@
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="30" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="17">
@@ -2534,13 +2544,13 @@
       <c r="E26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="40" t="s">
+      <c r="H26" s="31" t="s">
         <v>41</v>
       </c>
       <c r="I26" s="1"/>
@@ -2551,17 +2561,17 @@
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="17">
         <v>2</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="40"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -2570,17 +2580,17 @@
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
       <c r="D28" s="17">
         <v>3</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="40"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2589,17 +2599,17 @@
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="38"/>
-      <c r="C29" s="39"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="17">
         <v>4</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="40"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2608,15 +2618,15 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="38"/>
-      <c r="C30" s="39"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="17">
         <v>5</v>
       </c>
       <c r="E30" s="9"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="40"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -3281,6 +3291,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="H26:H30"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="B8:B12"/>
@@ -3290,21 +3315,6 @@
     <mergeCell ref="H8:H12"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="H26:H30"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="H14:H18"/>
   </mergeCells>
   <conditionalFormatting sqref="F8">
     <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="HIGH">

</xml_diff>